<commit_message>
VIMAS Custom Template Related Changes
</commit_message>
<xml_diff>
--- a/src/conf/ChargeBackMetadata.xlsx
+++ b/src/conf/ChargeBackMetadata.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="92">
   <si>
     <t>https://merituspayment.com/merchants/frmLogin.aspx</t>
   </si>
@@ -253,9 +253,6 @@
     <t>https://vimas.cynergydata.com/Vimas2.0/Login.aspx</t>
   </si>
   <si>
-    <t>10/20/2016</t>
-  </si>
-  <si>
     <t>10/27/2016</t>
   </si>
   <si>
@@ -280,10 +277,22 @@
     <t>https://vimas.cynergydata.com/Vimas2.0/Merchant/Report_Chargebacks.aspx</t>
   </si>
   <si>
-    <t>/wEPDwUJNTgwMDk2MzUyZBgBBQlHcmlkVmlldzEPPCsADAEIAgFkO749DL8/p3L9GZ04yuFdeFgaC3TrVqo5VrI5PHufMnU=</t>
-  </si>
-  <si>
-    <t>/wEWCwLAm+mdDQLlqpO0DwLM76k/AqzEjO8KAremvIMPApm9ztsKAuKX7J8MAoro7rgGAvqm5LULAtmm/tsBArGw/wg/bT8CxTDf6h2FxmKZ++S2A2mNAAvELCa5bRhj/DQAOQ==</t>
+    <t>Step4</t>
+  </si>
+  <si>
+    <t>Charge Back Details Get method</t>
+  </si>
+  <si>
+    <t>com.ibaseit.scraping.handler.VIMASExcelHandler</t>
+  </si>
+  <si>
+    <t>09/20/2016</t>
+  </si>
+  <si>
+    <t>?__VIEWSTATE</t>
+  </si>
+  <si>
+    <t>?__EVENTVALIDATION</t>
   </si>
 </sst>
 </file>
@@ -688,12 +697,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.25" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="255.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -930,7 +939,7 @@
         <v>57</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -938,7 +947,7 @@
         <v>58</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -970,7 +979,7 @@
         <v>63</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -984,7 +993,7 @@
         <v>65</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1020,7 +1029,7 @@
         <v>71</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1028,7 +1037,7 @@
         <v>72</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1060,16 +1069,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="136.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="136.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1205,7 +1214,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="A20" s="3"/>
       <c r="B20" s="1"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1219,7 +1228,7 @@
         <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1227,7 +1236,7 @@
         <v>15</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1235,7 +1244,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1251,123 +1260,188 @@
       <c r="B26" s="1"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>87</v>
+      <c r="A27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B28" s="1"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>88</v>
-      </c>
+      <c r="B29" s="1"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>78</v>
-      </c>
+      <c r="A30" s="3"/>
+      <c r="B30" s="1"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>79</v>
-      </c>
+      <c r="A31" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="1"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>33</v>
+        <v>7</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="7"/>
+        <v>15</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>36</v>
+        <v>1</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>43</v>
-      </c>
+      <c r="A35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="1"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>80</v>
-      </c>
+      <c r="A36" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="1"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="7"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="9"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="B47" s="9"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>45</v>
+      <c r="B48" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
-    <hyperlink ref="B23" r:id="rId3"/>
+    <hyperlink ref="B33" r:id="rId1"/>
+    <hyperlink ref="B23" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="200" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1418,74 +1492,6 @@
         <v>47</v>
       </c>
       <c r="E3" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="1">
         <v>5</v>
       </c>
     </row>
@@ -1497,10 +1503,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E3"/>
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1556,7 +1562,77 @@
         <v>5</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B15" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>